<commit_message>
PDF av komponentlise og milepælliste
</commit_message>
<xml_diff>
--- a/Gang og Sykkel varslingsystem/Komponentliste.xlsx
+++ b/Gang og Sykkel varslingsystem/Komponentliste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu.sharepoint.com/sites/o365_DugelegProsjekt/Shared Documents/General/Gang og Sykkel varslingsystem/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emile\Documents\Dugeleg\Gang og Sykkel varslingsystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="598" documentId="11_76A6F4E0D7503C526EF59792EBA098825550E92B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{557825D6-328E-4035-A78A-B5883D894972}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A22DC7-43D8-45CA-A002-DCFE552645E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -172,7 +172,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;kr&quot;\ * #,##0.00_-;\-&quot;kr&quot;\ * #,##0.00_-;_-&quot;kr&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;kr&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -704,13 +704,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B22" sqref="B1:G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" customWidth="1"/>
@@ -719,7 +722,7 @@
     <col min="7" max="7" width="62.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="109.5" customHeight="1">
+    <row r="1" spans="2:7" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -739,7 +742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="2:7">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
@@ -760,7 +763,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:7">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>9</v>
       </c>
@@ -781,7 +784,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
@@ -802,7 +805,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
         <v>15</v>
       </c>
@@ -820,7 +823,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
         <v>17</v>
       </c>
@@ -841,7 +844,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:7">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
         <v>20</v>
       </c>
@@ -862,7 +865,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:7">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>20</v>
       </c>
@@ -876,14 +879,14 @@
         <v>612.15</v>
       </c>
       <c r="F8" s="12">
-        <f>D8*E8</f>
+        <f t="shared" ref="F8:F13" si="1">D8*E8</f>
         <v>1224.3</v>
       </c>
       <c r="G8" s="13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="2:7">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
         <v>25</v>
       </c>
@@ -897,14 +900,14 @@
         <v>141.9</v>
       </c>
       <c r="F9" s="12">
-        <f>D9*E9</f>
+        <f t="shared" si="1"/>
         <v>283.8</v>
       </c>
       <c r="G9" s="13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="2:7">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
         <v>28</v>
       </c>
@@ -918,14 +921,14 @@
         <v>927.11940000000004</v>
       </c>
       <c r="F10" s="16">
-        <f>D10*E10</f>
+        <f t="shared" si="1"/>
         <v>1854.2388000000001</v>
       </c>
       <c r="G10" s="17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="2:7">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
         <v>31</v>
       </c>
@@ -939,14 +942,14 @@
         <v>183.7</v>
       </c>
       <c r="F11" s="12">
-        <f>D11*E11</f>
+        <f t="shared" si="1"/>
         <v>367.4</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:7">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
         <v>34</v>
       </c>
@@ -960,14 +963,14 @@
         <v>146.08000000000001</v>
       </c>
       <c r="F12" s="12">
-        <f>D12*E12</f>
+        <f t="shared" si="1"/>
         <v>292.16000000000003</v>
       </c>
       <c r="G12" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="2:7">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>37</v>
       </c>
@@ -981,14 +984,14 @@
         <v>30.16</v>
       </c>
       <c r="F13" s="16">
-        <f>D13*E13</f>
+        <f t="shared" si="1"/>
         <v>150.80000000000001</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>40</v>
       </c>
@@ -1006,7 +1009,7 @@
         <v>11551.728799999999</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="15" customHeight="1">
+    <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>41</v>
       </c>
@@ -1031,13 +1034,29 @@
     <hyperlink ref="G9" r:id="rId12" xr:uid="{A1B90D82-E655-4639-B49C-6F136B862A44}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="54" fitToHeight="0" orientation="landscape" r:id="rId13"/>
   <tableParts count="1">
-    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010063A40A4A8D2C6B4CA564D8EE51BC8BE9" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="23c42a97dd681451c13e7af1abeef51f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="db803184-edef-4b28-ac3d-3addf7576905" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2981854274215188bf3df9536b54658c" ns2:_="">
     <xsd:import namespace="db803184-edef-4b28-ac3d-3addf7576905"/>
@@ -1175,29 +1194,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA4953B4-0863-41C3-9103-173DB9CA391E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5B8CCA5-46C5-4FE2-8F8D-E0590993F707}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C585050-D745-4175-AE4B-4C2BE217B023}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C585050-D745-4175-AE4B-4C2BE217B023}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5B8CCA5-46C5-4FE2-8F8D-E0590993F707}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA4953B4-0863-41C3-9103-173DB9CA391E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="db803184-edef-4b28-ac3d-3addf7576905"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>